<commit_message>
Separated experiment script into experimental_lab.py
</commit_message>
<xml_diff>
--- a/benchmark/experiments/adding_headers_to_samples (soccer, rf@charfreq model, 100 runs per p_header value) [01-02-2017].xlsx
+++ b/benchmark/experiments/adding_headers_to_samples (soccer, rf@charfreq model, 100 runs per p_header value) [01-02-2017].xlsx
@@ -222,7 +222,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$22</c:f>
+              <c:f>Sheet1!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -294,7 +294,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$22</c:f>
+              <c:f>Sheet1!$D$3:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -374,11 +374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1130136032"/>
-        <c:axId val="1135926640"/>
+        <c:axId val="1201193312"/>
+        <c:axId val="1165950976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1130136032"/>
+        <c:axId val="1201193312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,6 +398,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -434,12 +435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1135926640"/>
+        <c:crossAx val="1165950976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1135926640"/>
+        <c:axId val="1165950976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +496,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1130136032"/>
+        <c:crossAx val="1201193312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1104,20 +1105,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1422,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1464,28 +1465,28 @@
         <v>100</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.74692307692307702</v>
+        <v>0.90909090909090751</v>
       </c>
       <c r="E2">
-        <v>3.5080617044005301E-2</v>
+        <v>1.5621425723676389E-15</v>
       </c>
       <c r="F2">
-        <v>0.68456196581196505</v>
+        <v>0.87878787878787668</v>
       </c>
       <c r="G2">
-        <v>4.14931279095739E-2</v>
+        <v>2.120050633927509E-15</v>
       </c>
       <c r="H2">
-        <v>0.82289661890397203</v>
+        <v>0.95454545454545359</v>
       </c>
       <c r="I2">
-        <v>1.8264136690259499E-2</v>
+        <v>1.0042345108077671E-15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1496,25 +1497,25 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.69769230769230794</v>
+        <v>0.74692307692307702</v>
       </c>
       <c r="E3">
-        <v>1.9725569228941801E-2</v>
+        <v>3.5080617044005301E-2</v>
       </c>
       <c r="F3">
-        <v>0.62625641025641099</v>
+        <v>0.68456196581196505</v>
       </c>
       <c r="G3">
-        <v>2.1821502081686098E-2</v>
+        <v>4.14931279095739E-2</v>
       </c>
       <c r="H3">
-        <v>0.80945177045176997</v>
+        <v>0.82289661890397203</v>
       </c>
       <c r="I3">
-        <v>1.0619185039878E-2</v>
+        <v>1.8264136690259499E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1525,25 +1526,25 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
-        <v>0.73230769230769199</v>
+        <v>0.69769230769230794</v>
       </c>
       <c r="E4">
-        <v>3.86243639668215E-2</v>
+        <v>1.9725569228941801E-2</v>
       </c>
       <c r="F4">
-        <v>0.65715384615384598</v>
+        <v>0.62625641025641099</v>
       </c>
       <c r="G4">
-        <v>4.5429135739773599E-2</v>
+        <v>2.1821502081686098E-2</v>
       </c>
       <c r="H4">
-        <v>0.82799816849816799</v>
+        <v>0.80945177045176997</v>
       </c>
       <c r="I4">
-        <v>2.03904820215738E-2</v>
+        <v>1.0619185039878E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1554,25 +1555,25 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
-        <v>0.74</v>
+        <v>0.73230769230769199</v>
       </c>
       <c r="E5">
-        <v>3.75255177857357E-2</v>
+        <v>3.86243639668215E-2</v>
       </c>
       <c r="F5">
-        <v>0.66348717948717995</v>
+        <v>0.65715384615384598</v>
       </c>
       <c r="G5">
-        <v>4.3701762002826501E-2</v>
+        <v>4.5429135739773599E-2</v>
       </c>
       <c r="H5">
-        <v>0.83042857142857096</v>
+        <v>0.82799816849816799</v>
       </c>
       <c r="I5">
-        <v>1.9080038001231401E-2</v>
+        <v>2.03904820215738E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1583,25 +1584,25 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D6">
-        <v>0.74076923076923096</v>
+        <v>0.74</v>
       </c>
       <c r="E6">
-        <v>3.73258913149161E-2</v>
+        <v>3.75255177857357E-2</v>
       </c>
       <c r="F6">
-        <v>0.66292307692307695</v>
+        <v>0.66348717948717995</v>
       </c>
       <c r="G6">
-        <v>4.2520705698972303E-2</v>
+        <v>4.3701762002826501E-2</v>
       </c>
       <c r="H6">
-        <v>0.83211446886446905</v>
+        <v>0.83042857142857096</v>
       </c>
       <c r="I6">
-        <v>1.8929057596011999E-2</v>
+        <v>1.9080038001231401E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1612,25 +1613,25 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.74538461538461498</v>
+        <v>0.74076923076923096</v>
       </c>
       <c r="E7">
-        <v>3.5755630670133202E-2</v>
+        <v>3.73258913149161E-2</v>
       </c>
       <c r="F7">
-        <v>0.66694871794871802</v>
+        <v>0.66292307692307695</v>
       </c>
       <c r="G7">
-        <v>4.2537062773559099E-2</v>
+        <v>4.2520705698972303E-2</v>
       </c>
       <c r="H7">
-        <v>0.83441666666666703</v>
+        <v>0.83211446886446905</v>
       </c>
       <c r="I7">
-        <v>1.8219480418637302E-2</v>
+        <v>1.8929057596011999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1641,25 +1642,25 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D8">
-        <v>0.72769230769230797</v>
+        <v>0.74538461538461498</v>
       </c>
       <c r="E8">
-        <v>3.85314050740026E-2</v>
+        <v>3.5755630670133202E-2</v>
       </c>
       <c r="F8">
-        <v>0.64623076923076905</v>
+        <v>0.66694871794871802</v>
       </c>
       <c r="G8">
-        <v>4.4664233008956097E-2</v>
+        <v>4.2537062773559099E-2</v>
       </c>
       <c r="H8">
-        <v>0.82450732600732601</v>
+        <v>0.83441666666666703</v>
       </c>
       <c r="I8">
-        <v>1.9701591649382399E-2</v>
+        <v>1.8219480418637302E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1670,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D9">
         <v>0.72769230769230797</v>
@@ -1679,16 +1680,16 @@
         <v>3.85314050740026E-2</v>
       </c>
       <c r="F9">
-        <v>0.64556410256410302</v>
+        <v>0.64623076923076905</v>
       </c>
       <c r="G9">
-        <v>4.4928709234304802E-2</v>
+        <v>4.4664233008956097E-2</v>
       </c>
       <c r="H9">
-        <v>0.82655067155067097</v>
+        <v>0.82450732600732601</v>
       </c>
       <c r="I9">
-        <v>2.0198877241479899E-2</v>
+        <v>1.9701591649382399E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1699,25 +1700,25 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D10">
-        <v>0.70923076923077</v>
+        <v>0.72769230769230797</v>
       </c>
       <c r="E10">
-        <v>3.2025630761017401E-2</v>
+        <v>3.85314050740026E-2</v>
       </c>
       <c r="F10">
-        <v>0.62466666666666704</v>
+        <v>0.64556410256410302</v>
       </c>
       <c r="G10">
-        <v>3.7507426705775303E-2</v>
+        <v>4.4928709234304802E-2</v>
       </c>
       <c r="H10">
-        <v>0.81665018315018301</v>
+        <v>0.82655067155067097</v>
       </c>
       <c r="I10">
-        <v>1.6760237619528998E-2</v>
+        <v>2.0198877241479899E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1728,25 +1729,25 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D11">
-        <v>0.70307692307692404</v>
+        <v>0.70923076923077</v>
       </c>
       <c r="E11">
-        <v>2.68257760015213E-2</v>
+        <v>3.2025630761017401E-2</v>
       </c>
       <c r="F11">
-        <v>0.61664102564102596</v>
+        <v>0.62466666666666704</v>
       </c>
       <c r="G11">
-        <v>3.18019204157763E-2</v>
+        <v>3.7507426705775303E-2</v>
       </c>
       <c r="H11">
-        <v>0.81370879120879103</v>
+        <v>0.81665018315018301</v>
       </c>
       <c r="I11">
-        <v>1.4431156672006E-2</v>
+        <v>1.6760237619528998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1757,25 +1758,25 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="D12">
-        <v>0.69846153846153902</v>
+        <v>0.70307692307692404</v>
       </c>
       <c r="E12">
-        <v>2.0973840334176201E-2</v>
+        <v>2.68257760015213E-2</v>
       </c>
       <c r="F12">
-        <v>0.61184615384615404</v>
+        <v>0.61664102564102596</v>
       </c>
       <c r="G12">
-        <v>2.4989867051720901E-2</v>
+        <v>3.18019204157763E-2</v>
       </c>
       <c r="H12">
-        <v>0.81226373626373605</v>
+        <v>0.81370879120879103</v>
       </c>
       <c r="I12">
-        <v>1.1905030009703299E-2</v>
+        <v>1.4431156672006E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1786,25 +1787,25 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="D13">
-        <v>0.69307692307692403</v>
+        <v>0.69846153846153902</v>
       </c>
       <c r="E13">
-        <v>7.6923076923076901E-3</v>
+        <v>2.0973840334176201E-2</v>
       </c>
       <c r="F13">
-        <v>0.60471794871794804</v>
+        <v>0.61184615384615404</v>
       </c>
       <c r="G13">
-        <v>9.9722351458661398E-3</v>
+        <v>2.4989867051720901E-2</v>
       </c>
       <c r="H13">
-        <v>0.80952747252747304</v>
+        <v>0.81226373626373605</v>
       </c>
       <c r="I13">
-        <v>7.0150348048514596E-3</v>
+        <v>1.1905030009703299E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1815,25 +1816,25 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D14">
         <v>0.69307692307692403</v>
       </c>
       <c r="E14">
-        <v>7.6923076923076997E-3</v>
+        <v>7.6923076923076901E-3</v>
       </c>
       <c r="F14">
-        <v>0.60579487179487201</v>
+        <v>0.60471794871794804</v>
       </c>
       <c r="G14">
-        <v>1.0635446311317799E-2</v>
+        <v>9.9722351458661398E-3</v>
       </c>
       <c r="H14">
-        <v>0.81075274725274704</v>
+        <v>0.80952747252747304</v>
       </c>
       <c r="I14">
-        <v>7.8272444499756805E-3</v>
+        <v>7.0150348048514596E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1844,25 +1845,25 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="D15">
-        <v>0.69230769230769296</v>
+        <v>0.69307692307692403</v>
       </c>
       <c r="E15">
-        <v>6.6948967387184501E-16</v>
+        <v>7.6923076923076997E-3</v>
       </c>
       <c r="F15">
-        <v>0.60648717948717901</v>
+        <v>0.60579487179487201</v>
       </c>
       <c r="G15">
-        <v>7.7177770530772304E-3</v>
+        <v>1.0635446311317799E-2</v>
       </c>
       <c r="H15">
-        <v>0.80955128205128202</v>
+        <v>0.81075274725274704</v>
       </c>
       <c r="I15">
-        <v>6.5127139547556303E-3</v>
+        <v>7.8272444499756805E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1873,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="D16">
         <v>0.69230769230769296</v>
@@ -1882,16 +1883,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F16">
-        <v>0.60887179487179499</v>
+        <v>0.60648717948717901</v>
       </c>
       <c r="G16">
-        <v>9.1723090529060407E-3</v>
+        <v>7.7177770530772304E-3</v>
       </c>
       <c r="H16">
-        <v>0.81041758241758299</v>
+        <v>0.80955128205128202</v>
       </c>
       <c r="I16">
-        <v>7.1488211461496597E-3</v>
+        <v>6.5127139547556303E-3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1902,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="D17">
         <v>0.69230769230769296</v>
@@ -1911,16 +1912,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F17">
-        <v>0.61110256410256403</v>
+        <v>0.60887179487179499</v>
       </c>
       <c r="G17">
-        <v>9.6495895109565098E-3</v>
+        <v>9.1723090529060407E-3</v>
       </c>
       <c r="H17">
-        <v>0.81126282051281995</v>
+        <v>0.81041758241758299</v>
       </c>
       <c r="I17">
-        <v>7.7070000195728202E-3</v>
+        <v>7.1488211461496597E-3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1931,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="D18">
         <v>0.69230769230769296</v>
@@ -1940,16 +1941,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F18">
-        <v>0.61243589743589799</v>
+        <v>0.61110256410256403</v>
       </c>
       <c r="G18">
-        <v>9.7203542524425899E-3</v>
+        <v>9.6495895109565098E-3</v>
       </c>
       <c r="H18">
-        <v>0.81083516483516505</v>
+        <v>0.81126282051281995</v>
       </c>
       <c r="I18">
-        <v>7.4948953410608797E-3</v>
+        <v>7.7070000195728202E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1960,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="D19">
         <v>0.69230769230769296</v>
@@ -1969,16 +1970,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F19">
-        <v>0.61543589743589799</v>
+        <v>0.61243589743589799</v>
       </c>
       <c r="G19">
-        <v>9.3768124115572293E-3</v>
+        <v>9.7203542524425899E-3</v>
       </c>
       <c r="H19">
-        <v>0.80907326007325997</v>
+        <v>0.81083516483516505</v>
       </c>
       <c r="I19">
-        <v>7.2740424000986301E-3</v>
+        <v>7.4948953410608797E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1989,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="D20">
         <v>0.69230769230769296</v>
@@ -1998,16 +1999,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F20">
-        <v>0.61961538461538501</v>
+        <v>0.61543589743589799</v>
       </c>
       <c r="G20">
-        <v>7.5693794998966E-3</v>
+        <v>9.3768124115572293E-3</v>
       </c>
       <c r="H20">
-        <v>0.80828388278388297</v>
+        <v>0.80907326007325997</v>
       </c>
       <c r="I20">
-        <v>7.6027597541207899E-3</v>
+        <v>7.2740424000986301E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2018,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="D21">
         <v>0.69230769230769296</v>
@@ -2027,16 +2028,16 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F21">
-        <v>0.62028205128205205</v>
+        <v>0.61961538461538501</v>
       </c>
       <c r="G21">
-        <v>6.32389376091381E-3</v>
+        <v>7.5693794998966E-3</v>
       </c>
       <c r="H21">
-        <v>0.80110714285714302</v>
+        <v>0.80828388278388297</v>
       </c>
       <c r="I21">
-        <v>9.2993792384829608E-3</v>
+        <v>7.6027597541207899E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2047,7 +2048,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D22">
         <v>0.69230769230769296</v>
@@ -2056,15 +2057,44 @@
         <v>6.6948967387184501E-16</v>
       </c>
       <c r="F22">
+        <v>0.62028205128205205</v>
+      </c>
+      <c r="G22">
+        <v>6.32389376091381E-3</v>
+      </c>
+      <c r="H22">
+        <v>0.80110714285714302</v>
+      </c>
+      <c r="I22">
+        <v>9.2993792384829608E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>100</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.69230769230769296</v>
+      </c>
+      <c r="E23">
+        <v>6.6948967387184501E-16</v>
+      </c>
+      <c r="F23">
         <v>0.62097435897436004</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>4.1613886839244303E-3</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>0.78995604395604402</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>5.8891216899316897E-3</v>
       </c>
     </row>

</xml_diff>